<commit_message>
Remove BRPSPTY values for 2018 and 2019
</commit_message>
<xml_diff>
--- a/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
+++ b/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS\Input Data for India 2.0\elec\BRPSPTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\elec\BRPSPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AB7B77-4490-4597-BFEE-CDDEDF1B8D10}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5730"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BRPSPTY" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>BRPSPTY BAU Renewable Portfolio Std Percentage This Year</t>
   </si>
@@ -74,12 +73,21 @@
   </si>
   <si>
     <t>RPS Fraction (dimensionless)</t>
+  </si>
+  <si>
+    <t>RPO national targets have historically not been achieved for wind and solar generation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The partial target achieved in 2018 &amp; 2019, is accounted in the real-world capacity deployed for  </t>
+  </si>
+  <si>
+    <t>wind and solar in elec/BPMCCS. Hence, we set the historical targets till 2019 to zero in this variable.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -295,23 +303,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -347,23 +338,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -539,25 +513,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" customWidth="1"/>
+    <col min="2" max="2" width="57.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -565,123 +539,138 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="8"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B51" s="4"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B52" s="4"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B53" s="4"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" s="1"/>
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
       <c r="B55" s="4"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
       <c r="B56" s="4"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" s="1"/>
       <c r="B57" s="4"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" s="1"/>
       <c r="B58" s="4"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
       <c r="B59" s="4"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{B2BAE028-4E3B-49D0-830C-E2072552B66B}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -690,22 +679,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -815,21 +804,21 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="5">
-        <v>0.115</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>0.14249999999999999</v>
+        <v>0</v>
       </c>
       <c r="D2" s="5">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="E2" s="5">
-        <v>0.17499999999999999</v>
+        <v>0</v>
       </c>
       <c r="F2" s="5">
         <v>0.19</v>

</xml_diff>

<commit_message>
WRI edit to BRPSPTY
</commit_message>
<xml_diff>
--- a/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
+++ b/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BRPSPTY" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -516,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -686,7 +686,7 @@
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="AI27" sqref="AI27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -821,17 +821,16 @@
         <v>0</v>
       </c>
       <c r="F2" s="5">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="G2" s="5">
         <v>0.19</v>
       </c>
-      <c r="G2" s="5">
-        <v>0.21</v>
-      </c>
       <c r="H2" s="5">
-        <f t="shared" ref="H2:AJ2" si="0">G2</f>
         <v>0.21</v>
       </c>
       <c r="I2" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I2:AJ2" si="0">H2</f>
         <v>0.21</v>
       </c>
       <c r="J2" s="5">

</xml_diff>

<commit_message>
Remove RPOs from BRPSPTY
</commit_message>
<xml_diff>
--- a/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
+++ b/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
@@ -15,7 +15,7 @@
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BRPSPTY" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>BRPSPTY BAU Renewable Portfolio Std Percentage This Year</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Note:</t>
   </si>
   <si>
-    <t>RPO trajectories are given by MoP till 2022 only, beyond which it is assumed constant at 2022 value</t>
-  </si>
-  <si>
     <t>The purpose of this variable is to specify the renewable portfolio standard</t>
   </si>
   <si>
@@ -69,19 +66,19 @@
     <t>via a policy lever, affecting the policy case).</t>
   </si>
   <si>
-    <t>India RPOs are differentiated by solar and non-solar.</t>
-  </si>
-  <si>
     <t>RPS Fraction (dimensionless)</t>
   </si>
   <si>
     <t>RPO national targets have historically not been achieved for wind and solar generation.</t>
   </si>
   <si>
-    <t xml:space="preserve">The partial target achieved in 2018 &amp; 2019, is accounted in the real-world capacity deployed for  </t>
-  </si>
-  <si>
-    <t>wind and solar in elec/BPMCCS. Hence, we set the historical targets till 2019 to zero in this variable.</t>
+    <t>Therefore, we do not include targets here, as we do not believe they are currently determining</t>
+  </si>
+  <si>
+    <t>capacity additions in the power sector. However, we do account for government renewable targets</t>
+  </si>
+  <si>
+    <t>in the variable elec/BPMCCS.</t>
   </si>
 </sst>
 </file>
@@ -514,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -584,17 +581,17 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
@@ -602,28 +599,26 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>17</v>
-      </c>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B51" s="4"/>
@@ -632,6 +627,7 @@
       <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A53" s="1"/>
       <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
@@ -656,16 +652,12 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
-      <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A62" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -686,7 +678,7 @@
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AI27" sqref="AI27"/>
+      <selection activeCell="B2" sqref="B2:AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -806,7 +798,7 @@
     </row>
     <row r="2" spans="1:36" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
@@ -821,125 +813,97 @@
         <v>0</v>
       </c>
       <c r="F2" s="5">
-        <v>0.17499999999999999</v>
+        <v>0</v>
       </c>
       <c r="G2" s="5">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="H2" s="5">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="I2" s="5">
-        <f t="shared" ref="I2:AJ2" si="0">H2</f>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="J2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="K2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="L2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="M2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="N2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="O2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="P2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="R2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="S2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="T2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="U2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="V2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="W2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="X2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="AB2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="AD2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="AF2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="AG2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="AH2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="AI2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="AJ2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.21</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>